<commit_message>
Case study with rcot multi-year capacity-expansion: infeasible but not in concept.xlsx
</commit_message>
<xml_diff>
--- a/default/3_sut_multi_year_rcot_cap - Copy/concept.xlsx
+++ b/default/3_sut_multi_year_rcot_cap - Copy/concept.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\pyesm\default\rcot_cap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\MIMO\pyESM\default\3_sut_multi_year_rcot_cap - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACED47B0-6779-48C8-8D77-37BB608B125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4C5E86-4E2D-4D68-A63B-AE6025B82267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio2" sheetId="2" r:id="rId1"/>
@@ -34,14 +34,14 @@
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">Foglio2!$J$24:$L$28</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="0" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,075"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,075"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Foglio2!$T$14</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""0,000001"""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""""</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
@@ -443,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
@@ -460,25 +460,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -759,10 +756,10 @@
   <dimension ref="A1:AH50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Y30" sqref="Y30"/>
+      <selection pane="bottomRight" activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,21 +873,21 @@
       <c r="N5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AF5" s="26" t="s">
+      <c r="AF5" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="T6" s="15" t="s">
+      <c r="T6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="Z6" s="15" t="s">
+      <c r="Z6" s="14" t="s">
         <v>46</v>
       </c>
       <c r="AF6" t="s">
@@ -937,20 +934,20 @@
       <c r="R7" s="3">
         <v>207</v>
       </c>
-      <c r="T7" s="14">
+      <c r="T7">
         <f t="array" ref="T7:X8">MMULT(AF7:AH8,TRANSPOSE(F24:H28))</f>
         <v>108.57763300759967</v>
       </c>
-      <c r="U7" s="14">
+      <c r="U7">
         <v>130.29315960911961</v>
       </c>
-      <c r="V7" s="14">
+      <c r="V7">
         <v>156.35179153094353</v>
       </c>
-      <c r="W7" s="14">
+      <c r="W7">
         <v>187.83930510314454</v>
       </c>
-      <c r="X7" s="14">
+      <c r="X7">
         <v>224.75570032572784</v>
       </c>
       <c r="Z7" s="13" cm="1">
@@ -1013,19 +1010,19 @@
       <c r="R8" s="3">
         <v>549899.56727395195</v>
       </c>
-      <c r="T8" s="14">
+      <c r="T8">
         <v>508022.2</v>
       </c>
-      <c r="U8" s="14">
+      <c r="U8">
         <v>518182.64399999997</v>
       </c>
-      <c r="V8" s="14">
+      <c r="V8">
         <v>528546.29688000004</v>
       </c>
-      <c r="W8" s="14">
+      <c r="W8">
         <v>539117.22281760001</v>
       </c>
-      <c r="X8" s="14">
+      <c r="X8">
         <v>549899.56727395195</v>
       </c>
       <c r="Z8" s="8">
@@ -1054,10 +1051,10 @@
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="Z9" s="15" t="s">
+      <c r="Z9" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1183,7 +1180,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="T13" s="15" t="s">
+      <c r="T13" s="14" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1194,7 +1191,7 @@
       <c r="E14" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I14" s="24" t="s">
         <v>43</v>
       </c>
       <c r="J14" s="2">
@@ -1206,10 +1203,10 @@
       <c r="L14" s="2">
         <v>5</v>
       </c>
-      <c r="S14" s="15" t="s">
+      <c r="S14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="T14" s="16">
+      <c r="T14" s="15">
         <f>SUM(R24:T28,R32:T36)</f>
         <v>2651862.1668773103</v>
       </c>
@@ -1221,7 +1218,7 @@
       <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="24" t="s">
         <v>44</v>
       </c>
       <c r="J15" s="2">
@@ -1241,7 +1238,7 @@
       <c r="E16" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="24" t="s">
         <v>45</v>
       </c>
       <c r="J16" s="2">
@@ -1261,7 +1258,7 @@
       <c r="E17" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="24" t="s">
         <v>56</v>
       </c>
       <c r="J17" s="2">
@@ -1278,7 +1275,7 @@
       <c r="E18" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="24" t="s">
         <v>57</v>
       </c>
       <c r="J18" s="2">
@@ -1298,7 +1295,7 @@
       <c r="E19" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="27" t="s">
+      <c r="I19" s="24" t="s">
         <v>59</v>
       </c>
       <c r="J19" s="2">
@@ -1312,17 +1309,17 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15" t="s">
+      <c r="I22" s="14"/>
+      <c r="J22" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="N22" s="15" t="s">
+      <c r="N22" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="R22" s="15" t="s">
+      <c r="R22" s="14" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1368,41 +1365,41 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="16">
         <v>108.57763300759967</v>
       </c>
-      <c r="G24" s="18">
-        <v>0</v>
-      </c>
-      <c r="H24" s="19">
+      <c r="G24" s="17">
+        <v>0</v>
+      </c>
+      <c r="H24" s="18">
         <v>508022.2</v>
       </c>
-      <c r="J24" s="17">
+      <c r="J24" s="16">
         <v>108.57763300759967</v>
       </c>
-      <c r="K24" s="18">
-        <v>0</v>
-      </c>
-      <c r="L24" s="19">
+      <c r="K24" s="17">
+        <v>0</v>
+      </c>
+      <c r="L24" s="18">
         <v>508022.2</v>
       </c>
-      <c r="N24" s="17">
+      <c r="N24" s="16">
         <v>1.7706724234768375E-2</v>
       </c>
-      <c r="O24" s="18">
-        <v>0</v>
-      </c>
-      <c r="P24" s="19">
+      <c r="O24" s="17">
+        <v>0</v>
+      </c>
+      <c r="P24" s="18">
         <v>2.8996700913242011</v>
       </c>
-      <c r="R24" s="14">
+      <c r="R24">
         <f t="array" ref="R24:T28">MMULT(N24:P28,_xlfn.MUNIT(3)*J14:L14)</f>
         <v>0.17706724234768376</v>
       </c>
-      <c r="S24" s="14">
-        <v>0</v>
-      </c>
-      <c r="T24" s="14">
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
         <v>14.498350456621004</v>
       </c>
     </row>
@@ -1410,40 +1407,40 @@
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="19">
         <v>130.29315960911961</v>
       </c>
-      <c r="G25" s="21">
-        <v>0</v>
-      </c>
-      <c r="H25" s="22">
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="20">
         <v>518182.64399999997</v>
       </c>
-      <c r="J25" s="20">
+      <c r="J25" s="19">
         <v>130.29315960911961</v>
       </c>
-      <c r="K25" s="21">
-        <v>0</v>
-      </c>
-      <c r="L25" s="22">
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+      <c r="L25" s="20">
         <v>518182.64399999997</v>
       </c>
-      <c r="N25" s="20">
+      <c r="N25" s="19">
         <v>3.5413448469536757E-3</v>
       </c>
-      <c r="O25" s="21">
-        <v>0</v>
-      </c>
-      <c r="P25" s="22">
+      <c r="O25" s="4">
+        <v>0</v>
+      </c>
+      <c r="P25" s="20">
         <v>5.7993401826483784E-2</v>
       </c>
-      <c r="R25" s="14">
+      <c r="R25">
         <v>3.5413448469536757E-2</v>
       </c>
-      <c r="S25" s="14">
-        <v>0</v>
-      </c>
-      <c r="T25" s="14">
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
         <v>0.28996700913241891</v>
       </c>
     </row>
@@ -1451,40 +1448,40 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="19">
         <v>156.35179153094353</v>
       </c>
-      <c r="G26" s="21">
-        <v>0</v>
-      </c>
-      <c r="H26" s="22">
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="20">
         <v>528546.29688000004</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="19">
         <v>156.35179153094353</v>
       </c>
-      <c r="K26" s="21">
-        <v>0</v>
-      </c>
-      <c r="L26" s="22">
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+      <c r="L26" s="20">
         <v>528546.29688000004</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="19">
         <v>4.2496138163444089E-3</v>
       </c>
-      <c r="O26" s="21">
-        <v>0</v>
-      </c>
-      <c r="P26" s="22">
+      <c r="O26" s="4">
+        <v>0</v>
+      </c>
+      <c r="P26" s="20">
         <v>0.181032667088767</v>
       </c>
-      <c r="R26" s="14">
+      <c r="R26">
         <v>4.2496138163444087E-2</v>
       </c>
-      <c r="S26" s="14">
-        <v>0</v>
-      </c>
-      <c r="T26" s="14">
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
         <v>0.90516333544383498</v>
       </c>
     </row>
@@ -1492,40 +1489,40 @@
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="19">
         <v>187.83930510314454</v>
       </c>
-      <c r="G27" s="21">
-        <v>0</v>
-      </c>
-      <c r="H27" s="22">
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="20">
         <v>539117.22281760001</v>
       </c>
-      <c r="J27" s="20">
+      <c r="J27" s="19">
         <v>187.83930510314454</v>
       </c>
-      <c r="K27" s="21">
-        <v>0</v>
-      </c>
-      <c r="L27" s="22">
+      <c r="K27" s="4">
+        <v>0</v>
+      </c>
+      <c r="L27" s="20">
         <v>539117.22281760001</v>
       </c>
-      <c r="N27" s="20">
+      <c r="N27" s="19">
         <v>5.1349500280823569E-3</v>
       </c>
-      <c r="O27" s="21">
-        <v>0</v>
-      </c>
-      <c r="P27" s="22">
-        <v>0</v>
-      </c>
-      <c r="R27" s="14">
+      <c r="O27" s="4">
+        <v>0</v>
+      </c>
+      <c r="P27" s="20">
+        <v>0</v>
+      </c>
+      <c r="R27">
         <v>5.1349500280823565E-2</v>
       </c>
-      <c r="S27" s="14">
-        <v>0</v>
-      </c>
-      <c r="T27" s="14">
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
         <v>0</v>
       </c>
     </row>
@@ -1533,94 +1530,93 @@
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="21">
         <v>224.75570032572784</v>
       </c>
-      <c r="G28" s="24">
-        <v>0</v>
-      </c>
-      <c r="H28" s="25">
+      <c r="G28" s="22">
+        <v>0</v>
+      </c>
+      <c r="H28" s="23">
         <v>549899.56727395195</v>
       </c>
-      <c r="J28" s="23">
+      <c r="J28" s="21">
         <v>224.75570032572784</v>
       </c>
-      <c r="K28" s="24">
-        <v>0</v>
-      </c>
-      <c r="L28" s="25">
+      <c r="K28" s="22">
+        <v>0</v>
+      </c>
+      <c r="L28" s="23">
         <v>549899.56727395195</v>
       </c>
-      <c r="N28" s="23">
+      <c r="N28" s="21">
         <v>6.0202862398211522E-3</v>
       </c>
-      <c r="O28" s="24">
-        <v>0</v>
-      </c>
-      <c r="P28" s="25">
-        <v>0</v>
-      </c>
-      <c r="R28" s="14">
+      <c r="O28" s="22">
+        <v>0</v>
+      </c>
+      <c r="P28" s="23">
+        <v>0</v>
+      </c>
+      <c r="R28">
         <v>6.0202862398211522E-2</v>
       </c>
-      <c r="S28" s="14">
-        <v>0</v>
-      </c>
-      <c r="T28" s="14">
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15" t="s">
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15" t="s">
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="S31" s="15"/>
+      <c r="S31" s="14"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="14">
+      <c r="J32">
         <f t="array" ref="J32:L36">N32:P36*J17:L17*8760</f>
         <v>0</v>
       </c>
-      <c r="K32" s="14">
-        <v>0</v>
-      </c>
-      <c r="L32" s="14">
-        <v>0</v>
-      </c>
-      <c r="N32" s="14">
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="N32">
         <f t="array" ref="N32:P36">J19:L19+MMULT(N46:R50,N24:P28)</f>
         <v>1.7706724234768375E-2</v>
       </c>
-      <c r="O32" s="14">
-        <v>0</v>
-      </c>
-      <c r="P32" s="14">
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
         <v>2.8996700913242011</v>
       </c>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14" cm="1">
-        <f t="array" ref="R32:T32">J24:L24*$J$15:$L$15</f>
+      <c r="R32">
+        <f t="array" ref="R32:T36">MMULT(J24:L28,_xlfn.MUNIT(3)*J15:L15)</f>
         <v>1085.7763300759966</v>
       </c>
-      <c r="S32" s="14">
-        <v>0</v>
-      </c>
-      <c r="T32" s="14">
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
         <v>508022.2</v>
       </c>
     </row>
@@ -1628,33 +1624,31 @@
       <c r="A33" t="s">
         <v>25</v>
       </c>
-      <c r="J33" s="14">
-        <v>0</v>
-      </c>
-      <c r="K33" s="14">
-        <v>0</v>
-      </c>
-      <c r="L33" s="14">
-        <v>0</v>
-      </c>
-      <c r="N33" s="14">
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="N33">
         <v>2.1248069081722051E-2</v>
       </c>
-      <c r="O33" s="14">
-        <v>0</v>
-      </c>
-      <c r="P33" s="14">
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
         <v>2.9576634931506849</v>
       </c>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14" cm="1">
-        <f t="array" ref="R33:T33">J25:L25*$J$15:$L$15</f>
+      <c r="R33">
         <v>1302.9315960911961</v>
       </c>
-      <c r="S33" s="14">
-        <v>0</v>
-      </c>
-      <c r="T33" s="14">
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
         <v>518182.64399999997</v>
       </c>
     </row>
@@ -1662,33 +1656,31 @@
       <c r="A34" t="s">
         <v>26</v>
       </c>
-      <c r="J34" s="14">
-        <v>0</v>
-      </c>
-      <c r="K34" s="14">
-        <v>0</v>
-      </c>
-      <c r="L34" s="14">
-        <v>0</v>
-      </c>
-      <c r="N34" s="14">
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="N34">
         <v>2.5497682898066459E-2</v>
       </c>
-      <c r="O34" s="14">
-        <v>0</v>
-      </c>
-      <c r="P34" s="14">
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
         <v>3.1386961602394519</v>
       </c>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14" cm="1">
-        <f t="array" ref="R34:T34">J26:L26*$J$15:$L$15</f>
+      <c r="R34">
         <v>1563.5179153094352</v>
       </c>
-      <c r="S34" s="14">
-        <v>0</v>
-      </c>
-      <c r="T34" s="14">
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
         <v>528546.29688000004</v>
       </c>
     </row>
@@ -1696,33 +1688,31 @@
       <c r="A35" t="s">
         <v>27</v>
       </c>
-      <c r="J35" s="14">
-        <v>0</v>
-      </c>
-      <c r="K35" s="14">
-        <v>0</v>
-      </c>
-      <c r="L35" s="14">
-        <v>0</v>
-      </c>
-      <c r="N35" s="14">
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="N35">
         <v>3.0632632926148817E-2</v>
       </c>
-      <c r="O35" s="14">
-        <v>0</v>
-      </c>
-      <c r="P35" s="14">
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
         <v>3.1386961602394519</v>
       </c>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14" cm="1">
-        <f t="array" ref="R35:T35">J27:L27*$J$15:$L$15</f>
+      <c r="R35">
         <v>1878.3930510314453</v>
       </c>
-      <c r="S35" s="14">
-        <v>0</v>
-      </c>
-      <c r="T35" s="14">
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
         <v>539117.22281760001</v>
       </c>
     </row>
@@ -1730,38 +1720,36 @@
       <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="J36" s="14">
-        <v>0</v>
-      </c>
-      <c r="K36" s="14">
-        <v>0</v>
-      </c>
-      <c r="L36" s="14">
-        <v>0</v>
-      </c>
-      <c r="N36" s="14">
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="N36">
         <v>3.6652919165969966E-2</v>
       </c>
-      <c r="O36" s="14">
-        <v>0</v>
-      </c>
-      <c r="P36" s="14">
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
         <v>3.1386961602394519</v>
       </c>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14" cm="1">
-        <f t="array" ref="R36:T36">J28:L28*$J$15:$L$15</f>
+      <c r="R36">
         <v>2247.5570032572787</v>
       </c>
-      <c r="S36" s="14">
-        <v>0</v>
-      </c>
-      <c r="T36" s="14">
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
         <v>549899.56727395195</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J38" s="15" t="s">
+      <c r="J38" s="14" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1769,14 +1757,14 @@
       <c r="A39" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="14">
+      <c r="J39">
         <f t="array" ref="J39:L43">N32:P36*J18:L18*8760</f>
         <v>108.57763300759967</v>
       </c>
-      <c r="K39" s="14">
-        <v>0</v>
-      </c>
-      <c r="L39" s="14">
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
         <v>508022.2</v>
       </c>
     </row>
@@ -1784,13 +1772,13 @@
       <c r="A40" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="14">
+      <c r="J40">
         <v>130.29315960911961</v>
       </c>
-      <c r="K40" s="14">
-        <v>0</v>
-      </c>
-      <c r="L40" s="14">
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
         <v>518182.64399999997</v>
       </c>
     </row>
@@ -1798,13 +1786,13 @@
       <c r="A41" t="s">
         <v>26</v>
       </c>
-      <c r="J41" s="14">
+      <c r="J41">
         <v>156.35179153094353</v>
       </c>
-      <c r="K41" s="14">
-        <v>0</v>
-      </c>
-      <c r="L41" s="14">
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
         <v>549899.56727395195</v>
       </c>
     </row>
@@ -1812,13 +1800,13 @@
       <c r="A42" t="s">
         <v>27</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J42">
         <v>187.83930510314451</v>
       </c>
-      <c r="K42" s="14">
-        <v>0</v>
-      </c>
-      <c r="L42" s="14">
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
         <v>549899.56727395195</v>
       </c>
     </row>
@@ -1826,18 +1814,18 @@
       <c r="A43" t="s">
         <v>28</v>
       </c>
-      <c r="J43" s="14">
+      <c r="J43">
         <v>224.75570032572782</v>
       </c>
-      <c r="K43" s="14">
-        <v>0</v>
-      </c>
-      <c r="L43" s="14">
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
         <v>549899.56727395195</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N45" s="15" t="s">
+      <c r="N45" s="14" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>